<commit_message>
Scheduling through properties file
</commit_message>
<xml_diff>
--- a/scan_report2022-03-29.xlsx
+++ b/scan_report2022-03-29.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="28">
   <si>
     <t>Sample Date</t>
   </si>
@@ -76,7 +76,28 @@
     <t>null</t>
   </si>
   <si>
+    <t>Foreign Matter Organic</t>
+  </si>
+  <si>
     <t>Foreign Matter Inorganic</t>
+  </si>
+  <si>
+    <t>Damaged Discoloured Sprouted And Weevilled Grains</t>
+  </si>
+  <si>
+    <t>Immature Shrunken And Shriveled Grains</t>
+  </si>
+  <si>
+    <t>Admixture Of Lower Class</t>
+  </si>
+  <si>
+    <t>Damaged Grains</t>
+  </si>
+  <si>
+    <t>Shriveled Immature Grains</t>
+  </si>
+  <si>
+    <t>Weevilled Grains</t>
   </si>
 </sst>
 </file>
@@ -252,7 +273,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -299,10 +320,25 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="O1" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2">
@@ -349,6 +385,21 @@
         <v>19</v>
       </c>
       <c r="O2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -359,7 +410,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -408,6 +459,27 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -450,6 +522,27 @@
         <v>19</v>
       </c>
       <c r="N2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U2" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>